<commit_message>
added .exe file that runs the conversion
</commit_message>
<xml_diff>
--- a/TransferList/ExcelToJson.xlsx
+++ b/TransferList/ExcelToJson.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PythonProjects\Jexcel\TransferList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36775E0-8DA8-4858-894E-9A0705264278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36370CD-BAD9-471C-87BE-BD2B0E18525C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1320" yWindow="4740" windowWidth="33450" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1320" yWindow="4740" windowWidth="26340" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,14 +59,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D:\PythonProjects\TestExcelToJson\New\1.json</t>
+    <t>D:\PythonProjects\TestExcelToJson\Json\1.json</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>D:\PythonProjects\TestExcelToJson\New\2.json</t>
-  </si>
-  <si>
-    <t>D:\PythonProjects\TestExcelToJson\New\3.json</t>
+    <t>D:\PythonProjects\TestExcelToJson\Json\2.json</t>
+  </si>
+  <si>
+    <t>D:\PythonProjects\TestExcelToJson\Json\3.json</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>